<commit_message>
Add the 'remove' method to 'SortedArray', not yet finished.
</commit_message>
<xml_diff>
--- a/doc/SortedArray_benchmark.xlsx
+++ b/doc/SortedArray_benchmark.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>n</t>
   </si>
@@ -63,14 +63,57 @@
     <t>60.6 MB</t>
   </si>
   <si>
-    <t>n is the number of elements int the container</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the number of elements in the container</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>t</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> is the time in ms to lookup 1'000'000 known elements + 1'000'000 unkown elements</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,16 +137,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -111,16 +168,86 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,9 +271,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="8.6266185476815402E-2"/>
-          <c:y val="0.18091462525517643"/>
-          <c:w val="0.62517825896762902"/>
-          <c:h val="0.68921660834062404"/>
+          <c:y val="7.9679984446388644E-2"/>
+          <c:w val="0.85594757386095965"/>
+          <c:h val="0.85217964421114023"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -156,7 +283,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$7</c:f>
+              <c:f>Sheet1!$AC$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -177,8 +304,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="6.6720253718285216E-2"/>
-                  <c:y val="0.32834463400408281"/>
+                  <c:x val="-0.2553982434887947"/>
+                  <c:y val="0.36603927286866922"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -186,7 +313,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$8:$M$27</c:f>
+              <c:f>Sheet1!$AB$8:$AB$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -255,7 +382,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$8:$N$27</c:f>
+              <c:f>Sheet1!$AC$8:$AC$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -354,7 +481,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.79556615519213947"/>
+          <c:y val="0.37754214056576263"/>
+          <c:w val="0.13254420994369978"/>
+          <c:h val="9.2250348871680293E-2"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -374,7 +510,17 @@
       <c:layout/>
     </c:title>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.842485431572277E-2"/>
+          <c:y val="0.1037031646460089"/>
+          <c:w val="0.8660244141586706"/>
+          <c:h val="0.83455523697245793"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -382,7 +528,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$7</c:f>
+              <c:f>Sheet1!$AP$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -403,8 +549,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-9.3722003499562556E-2"/>
-                  <c:y val="0.35149278215223095"/>
+                  <c:x val="-0.37053431126981884"/>
+                  <c:y val="0.4182525797953629"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -412,7 +558,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$X$8:$X$27</c:f>
+              <c:f>Sheet1!$AO$8:$AO$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -481,7 +627,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$Y$8:$Y$27</c:f>
+              <c:f>Sheet1!$AP$8:$AP$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -580,11 +726,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.72521046614687035"/>
+          <c:y val="0.38772895532235918"/>
+          <c:w val="0.15515930003039996"/>
+          <c:h val="0.13082665036556199"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -604,7 +755,17 @@
       <c:layout/>
     </c:title>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8552999502513168E-2"/>
+          <c:y val="0.1040879630305952"/>
+          <c:w val="0.87016279827766629"/>
+          <c:h val="0.83394134174786594"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -612,7 +773,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$AI$7</c:f>
+              <c:f>Sheet1!$BC$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -633,8 +794,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.10205533683289589"/>
-                  <c:y val="0.36075204141149025"/>
+                  <c:x val="-0.35789683152351054"/>
+                  <c:y val="0.42186259185134328"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -642,7 +803,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$AH$8:$AH$27</c:f>
+              <c:f>Sheet1!$BB$8:$BB$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -711,7 +872,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$AI$8:$AI$27</c:f>
+              <c:f>Sheet1!$BC$8:$BC$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -810,11 +971,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:legendEntry>
-        <c:idx val="1"/>
-        <c:delete val="1"/>
-      </c:legendEntry>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.71822551592815609"/>
+          <c:y val="0.37989121489683919"/>
+          <c:w val="0.16412742524831456"/>
+          <c:h val="0.13873324276023938"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -834,7 +1000,17 @@
       <c:layout/>
     </c:title>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.8681564149816793E-2"/>
+          <c:y val="0.1040879630305952"/>
+          <c:w val="0.8277450588725509"/>
+          <c:h val="0.83394134174786594"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -842,7 +1018,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$7</c:f>
+              <c:f>Sheet1!$P$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -872,7 +1048,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$8:$B$27</c:f>
+              <c:f>Sheet1!$O$8:$O$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -941,7 +1117,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$8:$C$27</c:f>
+              <c:f>Sheet1!$P$8:$P$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1040,7 +1216,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.82613193809039009"/>
+          <c:y val="0.40452592776552276"/>
+          <c:w val="0.14549926758336879"/>
+          <c:h val="8.9464011803719337E-2"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1060,7 +1245,17 @@
       <c:layout/>
     </c:title>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.2038264953722892E-2"/>
+          <c:y val="0.10373967466930115"/>
+          <c:w val="0.81047175024174611"/>
+          <c:h val="0.81593973170112211"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:ser>
@@ -1068,7 +1263,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$31</c:f>
+              <c:f>Sheet1!$C$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1098,7 +1293,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$32:$B$51</c:f>
+              <c:f>Sheet1!$B$8:$B$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1167,7 +1362,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$32:$C$51</c:f>
+              <c:f>Sheet1!$C$8:$C$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1266,7 +1461,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.80115122945158168"/>
+          <c:y val="0.39463098386124124"/>
+          <c:w val="0.14621719160104987"/>
+          <c:h val="8.9463994377846717E-2"/>
+        </c:manualLayout>
+      </c:layout>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -1282,16 +1486,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1312,16 +1516,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1342,16 +1546,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>35</xdr:col>
+      <xdr:col>55</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1372,16 +1576,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123824</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>457199</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1404,14 +1608,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1718,15 +1922,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AL52"/>
+  <dimension ref="B1:BF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AE24" sqref="AE24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:35" ht="18.75">
+    <row r="1" spans="2:58" ht="18.75">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1734,837 +1938,792 @@
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
     </row>
-    <row r="4" spans="2:35">
+    <row r="3" spans="2:58">
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="2:58">
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:35">
+    <row r="6" spans="2:58">
       <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="O6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
+      <c r="R6" t="s">
+        <v>8</v>
+      </c>
+      <c r="S6" t="s">
+        <v>9</v>
+      </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
-      <c r="X6" s="1" t="s">
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="AB6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AG6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AO6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Y6" s="1"/>
-      <c r="AH6" t="s">
+      <c r="AP6" s="1"/>
+      <c r="AR6" t="s">
+        <v>8</v>
+      </c>
+      <c r="AS6" t="s">
+        <v>12</v>
+      </c>
+      <c r="BB6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="BE6" t="s">
+        <v>8</v>
+      </c>
+      <c r="BF6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="7" spans="2:35">
-      <c r="B7" t="s">
+    <row r="7" spans="2:58">
+      <c r="B7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="M7" t="s">
+      <c r="O7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="N7" t="s">
+      <c r="P7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X7" t="s">
+      <c r="AB7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="Y7" t="s">
+      <c r="AC7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AO7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="AI7" t="s">
+      <c r="AP7" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="BB7" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="2:35">
-      <c r="B8">
+    <row r="8" spans="2:58">
+      <c r="B8" s="6">
         <v>9995</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="7">
+        <v>1891</v>
+      </c>
+      <c r="O8" s="6">
+        <v>9995</v>
+      </c>
+      <c r="P8" s="12">
         <v>1525</v>
       </c>
-      <c r="M8">
+      <c r="AB8" s="6">
         <v>9995</v>
       </c>
-      <c r="N8" s="2">
+      <c r="AC8" s="12">
         <v>1511</v>
       </c>
-      <c r="X8">
+      <c r="AO8" s="6">
         <v>9995</v>
       </c>
-      <c r="Y8">
+      <c r="AP8" s="7">
         <v>1588</v>
       </c>
-      <c r="AH8">
+      <c r="BB8" s="6">
         <v>9995</v>
       </c>
-      <c r="AI8">
+      <c r="BC8" s="7">
         <v>1646</v>
       </c>
     </row>
-    <row r="9" spans="2:35">
-      <c r="B9">
+    <row r="9" spans="2:58">
+      <c r="B9" s="8">
         <v>19982</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="9">
+        <v>2207</v>
+      </c>
+      <c r="O9" s="8">
+        <v>19982</v>
+      </c>
+      <c r="P9" s="9">
         <v>1681</v>
       </c>
-      <c r="M9">
+      <c r="AB9" s="8">
         <v>19982</v>
       </c>
-      <c r="N9">
+      <c r="AC9" s="9">
         <v>1666</v>
       </c>
-      <c r="X9">
+      <c r="AO9" s="8">
         <v>19982</v>
       </c>
-      <c r="Y9">
+      <c r="AP9" s="9">
         <v>1778</v>
       </c>
-      <c r="AH9">
+      <c r="BB9" s="8">
         <v>19982</v>
       </c>
-      <c r="AI9">
+      <c r="BC9" s="9">
         <v>1818</v>
       </c>
     </row>
-    <row r="10" spans="2:35">
-      <c r="B10">
+    <row r="10" spans="2:58">
+      <c r="B10" s="8">
         <v>29959</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="9">
+        <v>2433</v>
+      </c>
+      <c r="O10" s="8">
+        <v>29959</v>
+      </c>
+      <c r="P10" s="9">
         <v>1790</v>
       </c>
-      <c r="M10">
+      <c r="AB10" s="8">
         <v>29959</v>
       </c>
-      <c r="N10">
+      <c r="AC10" s="9">
         <v>1729</v>
       </c>
-      <c r="X10">
+      <c r="AO10" s="8">
         <v>29959</v>
       </c>
-      <c r="Y10">
+      <c r="AP10" s="9">
         <v>1922</v>
       </c>
-      <c r="AH10">
+      <c r="BB10" s="8">
         <v>29959</v>
       </c>
-      <c r="AI10">
+      <c r="BC10" s="9">
         <v>1929</v>
       </c>
     </row>
-    <row r="11" spans="2:35">
-      <c r="B11">
+    <row r="11" spans="2:58">
+      <c r="B11" s="8">
         <v>39931</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="9">
+        <v>2794</v>
+      </c>
+      <c r="O11" s="8">
+        <v>39931</v>
+      </c>
+      <c r="P11" s="9">
         <v>1876</v>
       </c>
-      <c r="M11">
+      <c r="AB11" s="8">
         <v>39931</v>
       </c>
-      <c r="N11">
+      <c r="AC11" s="9">
         <v>1842</v>
       </c>
-      <c r="X11">
+      <c r="AO11" s="8">
         <v>39931</v>
       </c>
-      <c r="Y11">
+      <c r="AP11" s="9">
         <v>1981</v>
       </c>
-      <c r="AH11">
+      <c r="BB11" s="8">
         <v>39931</v>
       </c>
-      <c r="AI11">
+      <c r="BC11" s="9">
         <v>2045</v>
       </c>
     </row>
-    <row r="12" spans="2:35">
-      <c r="B12">
+    <row r="12" spans="2:58">
+      <c r="B12" s="8">
         <v>49903</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="9">
+        <v>2959</v>
+      </c>
+      <c r="O12" s="8">
+        <v>49903</v>
+      </c>
+      <c r="P12" s="9">
         <v>1953</v>
       </c>
-      <c r="M12">
+      <c r="AB12" s="8">
         <v>49903</v>
       </c>
-      <c r="N12">
+      <c r="AC12" s="9">
         <v>1924</v>
       </c>
-      <c r="X12">
+      <c r="AO12" s="8">
         <v>49903</v>
       </c>
-      <c r="Y12">
+      <c r="AP12" s="9">
         <v>2071</v>
       </c>
-      <c r="AH12">
+      <c r="BB12" s="8">
         <v>49903</v>
       </c>
-      <c r="AI12">
+      <c r="BC12" s="9">
         <v>2077</v>
       </c>
     </row>
-    <row r="13" spans="2:35">
-      <c r="B13">
+    <row r="13" spans="2:58">
+      <c r="B13" s="8">
         <v>59844</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="9">
+        <v>2912</v>
+      </c>
+      <c r="O13" s="8">
+        <v>59844</v>
+      </c>
+      <c r="P13" s="9">
         <v>1971</v>
       </c>
-      <c r="M13">
+      <c r="AB13" s="8">
         <v>59844</v>
       </c>
-      <c r="N13">
+      <c r="AC13" s="9">
         <v>1958</v>
       </c>
-      <c r="X13">
+      <c r="AO13" s="8">
         <v>59844</v>
       </c>
-      <c r="Y13">
+      <c r="AP13" s="9">
         <v>2066</v>
       </c>
-      <c r="AH13">
+      <c r="BB13" s="8">
         <v>59844</v>
       </c>
-      <c r="AI13">
+      <c r="BC13" s="9">
         <v>2166</v>
       </c>
     </row>
-    <row r="14" spans="2:35">
-      <c r="B14">
+    <row r="14" spans="2:58">
+      <c r="B14" s="8">
         <v>69789</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="9">
+        <v>3099</v>
+      </c>
+      <c r="O14" s="8">
+        <v>69789</v>
+      </c>
+      <c r="P14" s="9">
         <v>1962</v>
       </c>
-      <c r="M14">
+      <c r="AB14" s="8">
         <v>69789</v>
       </c>
-      <c r="N14">
+      <c r="AC14" s="9">
         <v>2026</v>
       </c>
-      <c r="X14">
+      <c r="AO14" s="8">
         <v>69789</v>
       </c>
-      <c r="Y14">
+      <c r="AP14" s="9">
         <v>2169</v>
       </c>
-      <c r="AH14">
+      <c r="BB14" s="8">
         <v>69789</v>
       </c>
-      <c r="AI14">
+      <c r="BC14" s="9">
         <v>2192</v>
       </c>
     </row>
-    <row r="15" spans="2:35">
-      <c r="B15">
+    <row r="15" spans="2:58">
+      <c r="B15" s="8">
         <v>79712</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="9">
+        <v>3241</v>
+      </c>
+      <c r="O15" s="8">
+        <v>79712</v>
+      </c>
+      <c r="P15" s="9">
         <v>2001</v>
       </c>
-      <c r="M15">
+      <c r="AB15" s="8">
         <v>79712</v>
       </c>
-      <c r="N15">
+      <c r="AC15" s="9">
         <v>2093</v>
       </c>
-      <c r="X15">
+      <c r="AO15" s="8">
         <v>79712</v>
       </c>
-      <c r="Y15">
+      <c r="AP15" s="9">
         <v>2215</v>
       </c>
-      <c r="AH15">
+      <c r="BB15" s="8">
         <v>79712</v>
       </c>
-      <c r="AI15">
+      <c r="BC15" s="9">
         <v>2225</v>
       </c>
     </row>
-    <row r="16" spans="2:35">
-      <c r="B16">
+    <row r="16" spans="2:58">
+      <c r="B16" s="8">
         <v>89642</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="9">
+        <v>3452</v>
+      </c>
+      <c r="O16" s="8">
+        <v>89642</v>
+      </c>
+      <c r="P16" s="9">
         <v>2091</v>
       </c>
-      <c r="M16">
+      <c r="AB16" s="8">
         <v>89642</v>
       </c>
-      <c r="N16">
+      <c r="AC16" s="9">
         <v>2073</v>
       </c>
-      <c r="X16">
+      <c r="AO16" s="8">
         <v>89642</v>
       </c>
-      <c r="Y16">
+      <c r="AP16" s="9">
         <v>2291</v>
       </c>
-      <c r="AH16">
+      <c r="BB16" s="8">
         <v>89642</v>
       </c>
-      <c r="AI16">
+      <c r="BC16" s="9">
         <v>2259</v>
       </c>
     </row>
-    <row r="17" spans="2:38">
-      <c r="B17">
+    <row r="17" spans="2:55">
+      <c r="B17" s="8">
         <v>99568</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="9">
+        <v>3387</v>
+      </c>
+      <c r="O17" s="8">
+        <v>99568</v>
+      </c>
+      <c r="P17" s="9">
         <v>2121</v>
       </c>
-      <c r="M17">
+      <c r="AB17" s="8">
         <v>99568</v>
       </c>
-      <c r="N17">
+      <c r="AC17" s="9">
         <v>2099</v>
       </c>
-      <c r="X17">
+      <c r="AO17" s="8">
         <v>99568</v>
       </c>
-      <c r="Y17">
+      <c r="AP17" s="9">
         <v>2277</v>
       </c>
-      <c r="AH17">
+      <c r="BB17" s="8">
         <v>99568</v>
       </c>
-      <c r="AI17">
+      <c r="BC17" s="9">
         <v>2303</v>
       </c>
     </row>
-    <row r="18" spans="2:38">
-      <c r="B18">
+    <row r="18" spans="2:55">
+      <c r="B18" s="8">
         <v>109476</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="9">
+        <v>3338</v>
+      </c>
+      <c r="O18" s="8">
+        <v>109476</v>
+      </c>
+      <c r="P18" s="9">
         <v>2162</v>
       </c>
-      <c r="M18">
+      <c r="AB18" s="8">
         <v>109476</v>
       </c>
-      <c r="N18">
+      <c r="AC18" s="9">
         <v>2140</v>
       </c>
-      <c r="X18">
+      <c r="AO18" s="8">
         <v>109476</v>
       </c>
-      <c r="Y18">
+      <c r="AP18" s="9">
         <v>2301</v>
       </c>
-      <c r="AH18">
+      <c r="BB18" s="8">
         <v>109476</v>
       </c>
-      <c r="AI18">
+      <c r="BC18" s="9">
         <v>2338</v>
       </c>
     </row>
-    <row r="19" spans="2:38">
-      <c r="B19">
+    <row r="19" spans="2:55">
+      <c r="B19" s="8">
         <v>119367</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
+        <v>3504</v>
+      </c>
+      <c r="O19" s="8">
+        <v>119367</v>
+      </c>
+      <c r="P19" s="9">
         <v>2211</v>
       </c>
-      <c r="M19">
+      <c r="AB19" s="8">
         <v>119367</v>
       </c>
-      <c r="N19">
+      <c r="AC19" s="9">
         <v>2182</v>
       </c>
-      <c r="X19">
+      <c r="AO19" s="8">
         <v>119367</v>
       </c>
-      <c r="Y19">
+      <c r="AP19" s="9">
         <v>2362</v>
       </c>
-      <c r="AH19">
+      <c r="BB19" s="8">
         <v>119367</v>
       </c>
-      <c r="AI19">
+      <c r="BC19" s="9">
         <v>2371</v>
       </c>
     </row>
-    <row r="20" spans="2:38">
-      <c r="B20">
+    <row r="20" spans="2:55">
+      <c r="B20" s="8">
         <v>129263</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="9">
+        <v>3855</v>
+      </c>
+      <c r="O20" s="8">
+        <v>129263</v>
+      </c>
+      <c r="P20" s="9">
         <v>2229</v>
       </c>
-      <c r="M20">
+      <c r="AB20" s="8">
         <v>129263</v>
       </c>
-      <c r="N20">
+      <c r="AC20" s="9">
         <v>2258</v>
       </c>
-      <c r="X20">
+      <c r="AO20" s="8">
         <v>129263</v>
       </c>
-      <c r="Y20">
+      <c r="AP20" s="9">
         <v>2420</v>
       </c>
-      <c r="AH20">
+      <c r="BB20" s="8">
         <v>129263</v>
       </c>
-      <c r="AI20">
+      <c r="BC20" s="9">
         <v>2453</v>
       </c>
     </row>
-    <row r="21" spans="2:38">
-      <c r="B21">
+    <row r="21" spans="2:55">
+      <c r="B21" s="8">
         <v>139148</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="9">
+        <v>4052</v>
+      </c>
+      <c r="O21" s="8">
+        <v>139148</v>
+      </c>
+      <c r="P21" s="9">
         <v>2260</v>
       </c>
-      <c r="M21">
+      <c r="AB21" s="8">
         <v>139148</v>
       </c>
-      <c r="N21">
+      <c r="AC21" s="9">
         <v>2265</v>
       </c>
-      <c r="X21">
+      <c r="AO21" s="8">
         <v>139148</v>
       </c>
-      <c r="Y21">
+      <c r="AP21" s="9">
         <v>2513</v>
       </c>
-      <c r="AH21">
+      <c r="BB21" s="8">
         <v>139148</v>
       </c>
-      <c r="AI21">
+      <c r="BC21" s="9">
         <v>2489</v>
       </c>
     </row>
-    <row r="22" spans="2:38">
-      <c r="B22">
+    <row r="22" spans="2:55">
+      <c r="B22" s="8">
         <v>149025</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="9">
+        <v>4186</v>
+      </c>
+      <c r="O22" s="8">
+        <v>149025</v>
+      </c>
+      <c r="P22" s="9">
         <v>2315</v>
       </c>
-      <c r="M22">
+      <c r="AB22" s="8">
         <v>149025</v>
       </c>
-      <c r="N22">
+      <c r="AC22" s="9">
         <v>2334</v>
       </c>
-      <c r="X22">
+      <c r="AO22" s="8">
         <v>149025</v>
       </c>
-      <c r="Y22">
+      <c r="AP22" s="9">
         <v>2460</v>
       </c>
-      <c r="AH22">
+      <c r="BB22" s="8">
         <v>149025</v>
       </c>
-      <c r="AI22">
+      <c r="BC22" s="9">
         <v>2580</v>
       </c>
     </row>
-    <row r="23" spans="2:38">
-      <c r="B23">
+    <row r="23" spans="2:55">
+      <c r="B23" s="8">
         <v>158895</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="9">
+        <v>4320</v>
+      </c>
+      <c r="O23" s="8">
+        <v>158895</v>
+      </c>
+      <c r="P23" s="9">
         <v>2338</v>
       </c>
-      <c r="M23">
+      <c r="AB23" s="8">
         <v>158895</v>
       </c>
-      <c r="N23">
+      <c r="AC23" s="9">
         <v>2357</v>
       </c>
-      <c r="X23">
+      <c r="AO23" s="8">
         <v>158895</v>
       </c>
-      <c r="Y23">
+      <c r="AP23" s="9">
         <v>2515</v>
       </c>
-      <c r="AH23">
+      <c r="BB23" s="8">
         <v>158895</v>
       </c>
-      <c r="AI23">
+      <c r="BC23" s="9">
         <v>2554</v>
       </c>
     </row>
-    <row r="24" spans="2:38">
-      <c r="B24">
+    <row r="24" spans="2:55">
+      <c r="B24" s="8">
         <v>168768</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="9">
+        <v>4560</v>
+      </c>
+      <c r="O24" s="8">
+        <v>168768</v>
+      </c>
+      <c r="P24" s="9">
         <v>2360</v>
       </c>
-      <c r="M24">
+      <c r="AB24" s="8">
         <v>168768</v>
       </c>
-      <c r="N24">
+      <c r="AC24" s="9">
         <v>2402</v>
       </c>
-      <c r="X24">
+      <c r="AO24" s="8">
         <v>168768</v>
       </c>
-      <c r="Y24">
+      <c r="AP24" s="9">
         <v>2573</v>
       </c>
-      <c r="AH24">
+      <c r="BB24" s="8">
         <v>168768</v>
       </c>
-      <c r="AI24">
+      <c r="BC24" s="9">
         <v>2633</v>
       </c>
     </row>
-    <row r="25" spans="2:38">
-      <c r="B25">
+    <row r="25" spans="2:55">
+      <c r="B25" s="8">
         <v>178619</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="9">
+        <v>4663</v>
+      </c>
+      <c r="O25" s="8">
+        <v>178619</v>
+      </c>
+      <c r="P25" s="9">
         <v>2442</v>
       </c>
-      <c r="M25">
+      <c r="AB25" s="8">
         <v>178619</v>
       </c>
-      <c r="N25">
+      <c r="AC25" s="9">
         <v>2474</v>
       </c>
-      <c r="X25">
+      <c r="AO25" s="8">
         <v>178619</v>
       </c>
-      <c r="Y25">
+      <c r="AP25" s="9">
         <v>2639</v>
       </c>
-      <c r="AH25">
+      <c r="BB25" s="8">
         <v>178619</v>
       </c>
-      <c r="AI25">
+      <c r="BC25" s="9">
         <v>2664</v>
       </c>
     </row>
-    <row r="26" spans="2:38">
-      <c r="B26">
+    <row r="26" spans="2:55">
+      <c r="B26" s="8">
         <v>188458</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="9">
+        <v>4716</v>
+      </c>
+      <c r="O26" s="8">
+        <v>188458</v>
+      </c>
+      <c r="P26" s="9">
         <v>2428</v>
       </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" t="s">
-        <v>9</v>
-      </c>
-      <c r="M26">
+      <c r="AB26" s="8">
         <v>188458</v>
       </c>
-      <c r="N26">
+      <c r="AC26" s="9">
         <v>2448</v>
       </c>
-      <c r="P26" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>10</v>
-      </c>
-      <c r="X26">
+      <c r="AO26" s="8">
         <v>188458</v>
       </c>
-      <c r="Y26">
+      <c r="AP26" s="9">
         <v>2679</v>
       </c>
-      <c r="AA26" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB26" t="s">
-        <v>12</v>
-      </c>
-      <c r="AH26">
+      <c r="BB26" s="8">
         <v>188458</v>
       </c>
-      <c r="AI26">
+      <c r="BC26" s="9">
         <v>2714</v>
       </c>
-      <c r="AK26" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL26" t="s">
-        <v>13</v>
-      </c>
     </row>
-    <row r="27" spans="2:38">
-      <c r="B27">
+    <row r="27" spans="2:55">
+      <c r="B27" s="10">
         <v>198310</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="11">
+        <v>4719</v>
+      </c>
+      <c r="O27" s="10">
+        <v>198310</v>
+      </c>
+      <c r="P27" s="11">
         <v>2465</v>
       </c>
-      <c r="M27">
+      <c r="AB27" s="10">
         <v>198310</v>
       </c>
-      <c r="N27">
+      <c r="AC27" s="11">
         <v>2559</v>
       </c>
-      <c r="X27">
+      <c r="AO27" s="10">
         <v>198310</v>
       </c>
-      <c r="Y27">
+      <c r="AP27" s="11">
         <v>2647</v>
       </c>
-      <c r="AH27">
+      <c r="BB27" s="10">
         <v>198310</v>
       </c>
-      <c r="AI27">
+      <c r="BC27" s="11">
         <v>2769</v>
       </c>
     </row>
-    <row r="28" spans="2:38">
-      <c r="B28" t="s">
+    <row r="28" spans="2:55" s="5" customFormat="1">
+      <c r="B28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="5">
         <f>SUM(C8:C27) /COUNT(C8:C27)</f>
+        <v>3514.4</v>
+      </c>
+      <c r="O28" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P28" s="5">
+        <f>SUM(P8:P27) /COUNT(P8:P27)</f>
         <v>2109.0500000000002</v>
       </c>
-      <c r="M28" t="s">
+      <c r="AB28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="N28">
-        <f>SUM(N8:N27) /COUNT(N8:N27)</f>
+      <c r="AC28" s="5">
+        <f>SUM(AC8:AC27) /COUNT(AC8:AC27)</f>
         <v>2117</v>
       </c>
-      <c r="X28" t="s">
+      <c r="AO28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="Y28">
-        <f>SUM(Y8:Y27) /COUNT(Y8:Y27)</f>
+      <c r="AP28" s="5">
+        <f>SUM(AP8:AP27) /COUNT(AP8:AP27)</f>
         <v>2273.35</v>
       </c>
-      <c r="AH28" t="s">
+      <c r="BB28" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AI28">
-        <f>SUM(AI8:AI27) /COUNT(AI8:AI27)</f>
+      <c r="BC28" s="5">
+        <f>SUM(BC8:BC27) /COUNT(BC8:BC27)</f>
         <v>2311.25</v>
-      </c>
-    </row>
-    <row r="30" spans="2:38">
-      <c r="B30" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="31" spans="2:38">
-      <c r="B31" t="s">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="2:38">
-      <c r="B32">
-        <v>9995</v>
-      </c>
-      <c r="C32">
-        <v>1891</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33">
-        <v>19982</v>
-      </c>
-      <c r="C33">
-        <v>2207</v>
-      </c>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="B34">
-        <v>29959</v>
-      </c>
-      <c r="C34">
-        <v>2433</v>
-      </c>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35">
-        <v>39931</v>
-      </c>
-      <c r="C35">
-        <v>2794</v>
-      </c>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36">
-        <v>49903</v>
-      </c>
-      <c r="C36">
-        <v>2959</v>
-      </c>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="B37">
-        <v>59844</v>
-      </c>
-      <c r="C37">
-        <v>2912</v>
-      </c>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="B38">
-        <v>69789</v>
-      </c>
-      <c r="C38">
-        <v>3099</v>
-      </c>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39">
-        <v>79712</v>
-      </c>
-      <c r="C39">
-        <v>3241</v>
-      </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40">
-        <v>89642</v>
-      </c>
-      <c r="C40">
-        <v>3452</v>
-      </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41">
-        <v>99568</v>
-      </c>
-      <c r="C41">
-        <v>3387</v>
-      </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42">
-        <v>109476</v>
-      </c>
-      <c r="C42">
-        <v>3338</v>
-      </c>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43">
-        <v>119367</v>
-      </c>
-      <c r="C43">
-        <v>3504</v>
-      </c>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44">
-        <v>129263</v>
-      </c>
-      <c r="C44">
-        <v>3855</v>
-      </c>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="B45">
-        <v>139148</v>
-      </c>
-      <c r="C45">
-        <v>4052</v>
-      </c>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46">
-        <v>149025</v>
-      </c>
-      <c r="C46">
-        <v>4186</v>
-      </c>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47">
-        <v>158895</v>
-      </c>
-      <c r="C47">
-        <v>4320</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48">
-        <v>168768</v>
-      </c>
-      <c r="C48">
-        <v>4560</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6">
-      <c r="B49">
-        <v>178619</v>
-      </c>
-      <c r="C49">
-        <v>4663</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6">
-      <c r="B50">
-        <v>188458</v>
-      </c>
-      <c r="C50">
-        <v>4716</v>
-      </c>
-      <c r="E50" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6">
-      <c r="B51">
-        <v>198310</v>
-      </c>
-      <c r="C51">
-        <v>4719</v>
-      </c>
-    </row>
-    <row r="52" spans="2:6">
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52">
-        <f>SUM(C32:C51) /COUNT(C32:C51)</f>
-        <v>3514.4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>